<commit_message>
LOCAL: update import spreadsheet
</commit_message>
<xml_diff>
--- a/src/main/webapp/import/WildbookStandardFormatUpdated.xlsx
+++ b/src/main/webapp/import/WildbookStandardFormatUpdated.xlsx
@@ -456,10 +456,10 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="2" t="s">

</xml_diff>